<commit_message>
Rename TARGET to OWNER in DB Configuration file
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
+++ b/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F44969E-3F79-4F4F-9F70-5853F7D5100F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47920B0A-AD3B-4BC3-A354-EA3C85AECFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="23400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="C31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="C33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -51,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -75,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="G33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
   <si>
     <t>01_main_user_schema_sequence.sql</t>
   </si>
@@ -137,12 +137,6 @@
     <t>50_frontend_out_views.sql</t>
   </si>
   <si>
-    <t>GRANT_TRAGET_USER</t>
-  </si>
-  <si>
-    <t>TARGET_USER</t>
-  </si>
-  <si>
     <t>SEQ_NAME</t>
   </si>
   <si>
@@ -158,9 +152,6 @@
     <t>COPY_FUNC_NAME</t>
   </si>
   <si>
-    <t>TARGET_SCHEMA</t>
-  </si>
-  <si>
     <t>31_cds_in_to_db_log.sql</t>
   </si>
   <si>
@@ -176,12 +167,6 @@
     <t>16_cre_table_typ_log.sql</t>
   </si>
   <si>
-    <t>COPY_FUNC_SOURCE_SCHEMA</t>
-  </si>
-  <si>
-    <t>COPY_FUNC_SOURCE_TABLE_POSTFIX</t>
-  </si>
-  <si>
     <t>TABLE_PREFIX</t>
   </si>
   <si>
@@ -273,6 +258,24 @@
   </si>
   <si>
     <t>GRANT_TARGET_USER</t>
+  </si>
+  <si>
+    <t>OWNER_USER</t>
+  </si>
+  <si>
+    <t>OWNER_SCHEMA</t>
+  </si>
+  <si>
+    <t>SCHEMA_2</t>
+  </si>
+  <si>
+    <t>POSTFIX_2</t>
+  </si>
+  <si>
+    <t>SCHEMA_3</t>
+  </si>
+  <si>
+    <t>POSTFIX_3</t>
   </si>
 </sst>
 </file>
@@ -629,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,391 +645,418 @@
     <col min="3" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="I33" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K33" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="L33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" t="s">
         <v>23</v>
-      </c>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="2"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" t="s">
-        <v>28</v>
-      </c>
-      <c r="F34" t="s">
-        <v>2</v>
-      </c>
-      <c r="G34" t="s">
-        <v>29</v>
-      </c>
-      <c r="H34" t="s">
-        <v>3</v>
-      </c>
-      <c r="I34" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H35" t="s">
-        <v>3</v>
-      </c>
-      <c r="I35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" t="s">
-        <v>31</v>
-      </c>
-      <c r="D36" t="s">
-        <v>32</v>
       </c>
       <c r="F36" t="s">
         <v>2</v>
       </c>
       <c r="G36" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="H36" t="s">
         <v>3</v>
       </c>
       <c r="I36" t="s">
-        <v>31</v>
-      </c>
-      <c r="J36" t="s">
-        <v>8</v>
-      </c>
-      <c r="K36" t="s">
-        <v>19</v>
-      </c>
-      <c r="L36" t="s">
-        <v>28</v>
-      </c>
-      <c r="M36" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H37" t="s">
         <v>3</v>
       </c>
       <c r="I37" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" t="s">
         <v>27</v>
       </c>
-      <c r="D38" t="s">
+      <c r="F38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G38" t="s">
         <v>28</v>
       </c>
       <c r="H38" t="s">
         <v>3</v>
       </c>
       <c r="I38" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="J38" t="s">
+        <v>8</v>
+      </c>
+      <c r="K38" t="s">
+        <v>16</v>
+      </c>
+      <c r="L38" t="s">
+        <v>23</v>
+      </c>
+      <c r="M38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H39" t="s">
         <v>3</v>
       </c>
       <c r="I39" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" t="s">
         <v>22</v>
       </c>
-      <c r="C40" t="s">
-        <v>31</v>
-      </c>
       <c r="D40" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="H40" t="s">
         <v>3</v>
       </c>
       <c r="I40" t="s">
-        <v>31</v>
-      </c>
-      <c r="J40" t="s">
-        <v>18</v>
-      </c>
-      <c r="K40" t="s">
-        <v>20</v>
-      </c>
-      <c r="L40" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H41" t="s">
         <v>3</v>
       </c>
       <c r="I41" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" t="s">
+        <v>27</v>
+      </c>
       <c r="H42" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I42" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>6</v>
-      </c>
-      <c r="C43" t="s">
-        <v>27</v>
-      </c>
-      <c r="D43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E43" t="s">
-        <v>7</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="J42" t="s">
+        <v>15</v>
+      </c>
+      <c r="K42" t="s">
+        <v>17</v>
+      </c>
+      <c r="L42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H43" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I43" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H44" t="s">
         <v>5</v>
       </c>
       <c r="I44" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" t="s">
+        <v>29</v>
+      </c>
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" t="s">
+        <v>5</v>
+      </c>
+      <c r="I45" t="s">
+        <v>22</v>
+      </c>
+      <c r="L45" t="s">
+        <v>23</v>
+      </c>
+      <c r="M45" t="s">
+        <v>2</v>
+      </c>
+      <c r="N45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H46" t="s">
+        <v>5</v>
+      </c>
+      <c r="I46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rename DB Definition Columns in Excel File
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
+++ b/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F80C358-B27D-4B8F-A418-93CE2263B9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38361CB9-133F-4CD5-85A8-FAA0C1735CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="23400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="59">
   <si>
     <t>01_main_user_schema_sequence.sql</t>
   </si>
@@ -276,6 +276,12 @@
   </si>
   <si>
     <t>POSTFIX_3</t>
+  </si>
+  <si>
+    <t>TABLE_POSTFIX_2</t>
+  </si>
+  <si>
+    <t>TABLE_POSTFIX_3</t>
   </si>
 </sst>
 </file>
@@ -635,7 +641,7 @@
   <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,7 +655,10 @@
     <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -858,13 +867,13 @@
         <v>53</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>55</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -1037,9 +1046,6 @@
       </c>
       <c r="M45" t="s">
         <v>2</v>
-      </c>
-      <c r="N45" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add Generating Create View SQL Scripts
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
+++ b/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38361CB9-133F-4CD5-85A8-FAA0C1735CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA863374-EC04-4701-8766-5FEBBE9C3511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="23400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autor:</t>
         </r>
@@ -42,7 +42,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 GRANT TRIGGER
@@ -59,7 +59,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autor:</t>
         </r>
@@ -68,7 +68,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Rawdaten = varchar oder kein Eintrag dann Datentypen</t>
@@ -83,7 +83,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autor:</t>
         </r>
@@ -92,7 +92,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Sequenz immer an die Spalte [Resource]_[Postfix]_id mit ALTER TABLE / GRANT USAGE ON seq to USER
@@ -301,13 +301,13 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Segoe UI"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Segoe UI"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -641,7 +641,7 @@
   <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add raw id column and an own sequence to typed tables
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
+++ b/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA863374-EC04-4701-8766-5FEBBE9C3511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE2F8EE-262C-4677-B5F7-3D7561216783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="59">
   <si>
     <t>01_main_user_schema_sequence.sql</t>
   </si>
@@ -641,7 +641,7 @@
   <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,6 +965,9 @@
       <c r="D40" t="s">
         <v>23</v>
       </c>
+      <c r="G40" t="s">
+        <v>24</v>
+      </c>
       <c r="H40" t="s">
         <v>3</v>
       </c>
@@ -989,6 +992,9 @@
       </c>
       <c r="D42" t="s">
         <v>27</v>
+      </c>
+      <c r="G42" t="s">
+        <v>28</v>
       </c>
       <c r="H42" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Correction of the copy function and creation of the necessary views for the data processor
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
+++ b/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE2F8EE-262C-4677-B5F7-3D7561216783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640"/>
   </bookViews>
   <sheets>
     <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,12 +19,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="C33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="C33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="F33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -75,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="G33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -105,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
   <si>
     <t>01_main_user_schema_sequence.sql</t>
   </si>
@@ -282,12 +281,24 @@
   </si>
   <si>
     <t>TABLE_POSTFIX_3</t>
+  </si>
+  <si>
+    <t>19_cre_view_type_datap_all</t>
+  </si>
+  <si>
+    <t>_all_data</t>
+  </si>
+  <si>
+    <t>db2dataprocessor_user</t>
+  </si>
+  <si>
+    <t>db2dataprocessor_out</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -637,11 +648,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,6 +1075,29 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" t="s">
+        <v>62</v>
+      </c>
+      <c r="E47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" t="s">
+        <v>60</v>
+      </c>
+      <c r="H47" t="s">
+        <v>5</v>
+      </c>
+      <c r="I47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rename file and reference to this file
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
+++ b/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A2CC36-D624-4434-972F-A956AE91B2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640"/>
+    <workbookView xWindow="12495" yWindow="8955" windowWidth="25905" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
@@ -19,12 +20,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="C33" authorId="0" shapeId="0">
+    <comment ref="C33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -50,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="0" shapeId="0">
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G33" authorId="0" shapeId="0">
+    <comment ref="G33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -283,9 +284,6 @@
     <t>TABLE_POSTFIX_3</t>
   </si>
   <si>
-    <t>19_cre_view_type_datap_all</t>
-  </si>
-  <si>
     <t>_all_data</t>
   </si>
   <si>
@@ -293,12 +291,15 @@
   </si>
   <si>
     <t>db2dataprocessor_out</t>
+  </si>
+  <si>
+    <t>19_cre_view_typ_dataproc_all</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -648,11 +649,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,25 +1076,25 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C47" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" t="s">
         <v>61</v>
-      </c>
-      <c r="D47" t="s">
-        <v>62</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
       </c>
       <c r="F47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H47" t="s">
         <v>5</v>
       </c>
       <c r="I47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Generate DB View SQL files for Dataprocessor all tables
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
+++ b/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A2CC36-D624-4434-972F-A956AE91B2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1507B542-A8C4-4660-865A-24118F43E277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12495" yWindow="8955" windowWidth="25905" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="255" yWindow="2250" windowWidth="25905" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="66">
   <si>
     <t>01_main_user_schema_sequence.sql</t>
   </si>
@@ -293,7 +293,16 @@
     <t>db2dataprocessor_out</t>
   </si>
   <si>
-    <t>19_cre_view_typ_dataproc_all</t>
+    <t>template_cre_table.sql</t>
+  </si>
+  <si>
+    <t>template_cre_view.sql</t>
+  </si>
+  <si>
+    <t>template_cre_view2.sql</t>
+  </si>
+  <si>
+    <t>19_cre_view_typ_dataproc_all.sql</t>
   </si>
 </sst>
 </file>
@@ -653,14 +662,15 @@
   <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
@@ -897,6 +907,9 @@
       <c r="A36" t="s">
         <v>1</v>
       </c>
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
       <c r="C36" t="s">
         <v>22</v>
       </c>
@@ -928,6 +941,9 @@
       <c r="A38" t="s">
         <v>4</v>
       </c>
+      <c r="B38" t="s">
+        <v>62</v>
+      </c>
       <c r="C38" t="s">
         <v>26</v>
       </c>
@@ -971,6 +987,9 @@
       <c r="A40" t="s">
         <v>18</v>
       </c>
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
       <c r="C40" t="s">
         <v>22</v>
       </c>
@@ -999,6 +1018,9 @@
       <c r="A42" t="s">
         <v>19</v>
       </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
       <c r="C42" t="s">
         <v>26</v>
       </c>
@@ -1044,6 +1066,9 @@
       <c r="A45" t="s">
         <v>6</v>
       </c>
+      <c r="B45" t="s">
+        <v>63</v>
+      </c>
       <c r="C45" t="s">
         <v>22</v>
       </c>
@@ -1076,7 +1101,10 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>65</v>
+      </c>
+      <c r="B47" t="s">
+        <v>64</v>
       </c>
       <c r="C47" t="s">
         <v>60</v>
@@ -1095,6 +1123,9 @@
       </c>
       <c r="I47" t="s">
         <v>60</v>
+      </c>
+      <c r="L47" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Remove DB View from Version 0.1.0
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
+++ b/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1507B542-A8C4-4660-865A-24118F43E277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301BF2D3-2228-445D-B07A-00C1A60BB831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="2250" windowWidth="25905" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="705" windowWidth="25200" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="65">
   <si>
     <t>01_main_user_schema_sequence.sql</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>30_cds_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t>50_frontend_out_views.sql</t>
   </si>
   <si>
     <t>SEQ_NAME</t>
@@ -659,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O48"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,217 +682,217 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" s="2"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="J33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L33" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="M33" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O33" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -908,25 +905,25 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" t="s">
         <v>22</v>
-      </c>
-      <c r="D36" t="s">
-        <v>23</v>
       </c>
       <c r="F36" t="s">
         <v>2</v>
       </c>
       <c r="G36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H36" t="s">
         <v>3</v>
       </c>
       <c r="I36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -934,7 +931,7 @@
         <v>3</v>
       </c>
       <c r="I37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -942,34 +939,34 @@
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" t="s">
         <v>26</v>
-      </c>
-      <c r="D38" t="s">
-        <v>27</v>
       </c>
       <c r="F38" t="s">
         <v>2</v>
       </c>
       <c r="G38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H38" t="s">
         <v>3</v>
       </c>
       <c r="I38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J38" t="s">
         <v>8</v>
       </c>
       <c r="K38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M38" t="s">
         <v>2</v>
@@ -980,30 +977,30 @@
         <v>3</v>
       </c>
       <c r="I39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" t="s">
         <v>22</v>
       </c>
-      <c r="D40" t="s">
+      <c r="G40" t="s">
         <v>23</v>
-      </c>
-      <c r="G40" t="s">
-        <v>24</v>
       </c>
       <c r="H40" t="s">
         <v>3</v>
       </c>
       <c r="I40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
@@ -1011,39 +1008,39 @@
         <v>3</v>
       </c>
       <c r="I41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C42" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" t="s">
         <v>26</v>
       </c>
-      <c r="D42" t="s">
+      <c r="G42" t="s">
         <v>27</v>
-      </c>
-      <c r="G42" t="s">
-        <v>28</v>
       </c>
       <c r="H42" t="s">
         <v>3</v>
       </c>
       <c r="I42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -1051,7 +1048,7 @@
         <v>3</v>
       </c>
       <c r="I43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
@@ -1059,7 +1056,7 @@
         <v>5</v>
       </c>
       <c r="I44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -1067,13 +1064,13 @@
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E45" t="s">
         <v>7</v>
@@ -1082,10 +1079,10 @@
         <v>5</v>
       </c>
       <c r="I45" t="s">
+        <v>21</v>
+      </c>
+      <c r="L45" t="s">
         <v>22</v>
-      </c>
-      <c r="L45" t="s">
-        <v>23</v>
       </c>
       <c r="M45" t="s">
         <v>2</v>
@@ -1096,41 +1093,36 @@
         <v>5</v>
       </c>
       <c r="I46" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C47" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" t="s">
         <v>60</v>
-      </c>
-      <c r="D47" t="s">
-        <v>61</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
       </c>
       <c r="F47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H47" t="s">
         <v>5</v>
       </c>
       <c r="I47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L47" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update create view statements
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
+++ b/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301BF2D3-2228-445D-B07A-00C1A60BB831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C693A73E-A5E3-4817-BF91-BB803490F9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="705" windowWidth="25200" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
   <si>
     <t>01_main_user_schema_sequence.sql</t>
   </si>
@@ -658,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,10 +1082,13 @@
         <v>21</v>
       </c>
       <c r="L45" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="M45" t="s">
         <v>2</v>
+      </c>
+      <c r="N45" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
DB Config: provide a summary of database jobs
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
+++ b/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C693A73E-A5E3-4817-BF91-BB803490F9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640"/>
   </bookViews>
   <sheets>
     <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
@@ -20,12 +19,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="C33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="C33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="F33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -75,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="G33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -105,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="66">
   <si>
     <t>01_main_user_schema_sequence.sql</t>
   </si>
@@ -281,9 +280,6 @@
     <t>TABLE_POSTFIX_3</t>
   </si>
   <si>
-    <t>_all_data</t>
-  </si>
-  <si>
     <t>db2dataprocessor_user</t>
   </si>
   <si>
@@ -300,12 +296,18 @@
   </si>
   <si>
     <t>19_cre_view_typ_dataproc_all.sql</t>
+  </si>
+  <si>
+    <t>02_db_config_tools.sql</t>
+  </si>
+  <si>
+    <t>_all</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -655,11 +657,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,12 +902,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C36" t="s">
         <v>21</v>
@@ -939,7 +946,7 @@
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C38" t="s">
         <v>25</v>
@@ -985,7 +992,7 @@
         <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
         <v>21</v>
@@ -1016,7 +1023,7 @@
         <v>18</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" t="s">
         <v>25</v>
@@ -1064,7 +1071,7 @@
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C45" t="s">
         <v>21</v>
@@ -1101,28 +1108,28 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C47" t="s">
+        <v>58</v>
+      </c>
+      <c r="D47" t="s">
         <v>59</v>
-      </c>
-      <c r="D47" t="s">
-        <v>60</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
       </c>
       <c r="F47" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="H47" t="s">
         <v>5</v>
       </c>
       <c r="I47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L47" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Remove templates for unchanged generated files
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
+++ b/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BE378C-3D61-40A1-B77E-54E64AB91BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
@@ -19,12 +20,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="C33" authorId="0" shapeId="0">
+    <comment ref="C33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -50,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="0" shapeId="0">
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G33" authorId="0" shapeId="0">
+    <comment ref="G33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -104,10 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="66">
-  <si>
-    <t>01_main_user_schema_sequence.sql</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
   <si>
     <t>10_cre_table_raw_cds2db_in.sql</t>
   </si>
@@ -296,9 +294,6 @@
   </si>
   <si>
     <t>19_cre_view_typ_dataproc_all.sql</t>
-  </si>
-  <si>
-    <t>02_db_config_tools.sql</t>
   </si>
   <si>
     <t>_all</t>
@@ -307,7 +302,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -657,11 +652,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+      <selection activeCell="A34" sqref="A34:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,307 +679,328 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="2"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="J33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L33" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="M33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O33" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
+      <c r="B34" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" t="s">
+        <v>2</v>
+      </c>
+      <c r="I34" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>64</v>
+      <c r="H35" t="s">
+        <v>2</v>
+      </c>
+      <c r="I35" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" t="s">
         <v>1</v>
       </c>
-      <c r="B36" t="s">
-        <v>60</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="G36" t="s">
+        <v>26</v>
+      </c>
+      <c r="H36" t="s">
+        <v>2</v>
+      </c>
+      <c r="I36" t="s">
+        <v>24</v>
+      </c>
+      <c r="J36" t="s">
+        <v>7</v>
+      </c>
+      <c r="K36" t="s">
+        <v>14</v>
+      </c>
+      <c r="L36" t="s">
         <v>21</v>
       </c>
-      <c r="D36" t="s">
-        <v>22</v>
-      </c>
-      <c r="F36" t="s">
-        <v>2</v>
-      </c>
-      <c r="G36" t="s">
-        <v>23</v>
-      </c>
-      <c r="H36" t="s">
-        <v>3</v>
-      </c>
-      <c r="I36" t="s">
-        <v>21</v>
+      <c r="M36" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D38" t="s">
-        <v>26</v>
-      </c>
-      <c r="F38" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" t="s">
+        <v>22</v>
+      </c>
+      <c r="H38" t="s">
         <v>2</v>
       </c>
-      <c r="G38" t="s">
-        <v>27</v>
-      </c>
-      <c r="H38" t="s">
-        <v>3</v>
-      </c>
       <c r="I38" t="s">
-        <v>25</v>
-      </c>
-      <c r="J38" t="s">
-        <v>8</v>
-      </c>
-      <c r="K38" t="s">
-        <v>15</v>
-      </c>
-      <c r="L38" t="s">
-        <v>22</v>
-      </c>
-      <c r="M38" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
@@ -992,147 +1008,116 @@
         <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C40" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D40" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G40" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I40" t="s">
+        <v>24</v>
+      </c>
+      <c r="J40" t="s">
+        <v>13</v>
+      </c>
+      <c r="K40" t="s">
+        <v>15</v>
+      </c>
+      <c r="L40" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>18</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="H42" t="s">
+        <v>4</v>
+      </c>
+      <c r="I42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" t="s">
         <v>60</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
+      <c r="H43" t="s">
+        <v>4</v>
+      </c>
+      <c r="I43" t="s">
+        <v>20</v>
+      </c>
+      <c r="L43" t="s">
         <v>25</v>
       </c>
-      <c r="D42" t="s">
-        <v>26</v>
-      </c>
-      <c r="G42" t="s">
-        <v>27</v>
-      </c>
-      <c r="H42" t="s">
-        <v>3</v>
-      </c>
-      <c r="I42" t="s">
-        <v>25</v>
-      </c>
-      <c r="J42" t="s">
-        <v>14</v>
-      </c>
-      <c r="K42" t="s">
-        <v>16</v>
-      </c>
-      <c r="L42" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H43" t="s">
-        <v>3</v>
-      </c>
-      <c r="I43" t="s">
-        <v>24</v>
+      <c r="M43" t="s">
+        <v>1</v>
+      </c>
+      <c r="N43" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I44" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="B45" t="s">
         <v>61</v>
       </c>
       <c r="C45" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="D45" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="E45" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="F45" t="s">
+        <v>63</v>
       </c>
       <c r="H45" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I45" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="L45" t="s">
-        <v>26</v>
-      </c>
-      <c r="M45" t="s">
-        <v>2</v>
-      </c>
-      <c r="N45" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H46" t="s">
-        <v>5</v>
-      </c>
-      <c r="I46" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>63</v>
-      </c>
-      <c r="B47" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47" t="s">
-        <v>58</v>
-      </c>
-      <c r="D47" t="s">
-        <v>59</v>
-      </c>
-      <c r="E47" t="s">
-        <v>7</v>
-      </c>
-      <c r="F47" t="s">
-        <v>65</v>
-      </c>
-      <c r="H47" t="s">
-        <v>5</v>
-      </c>
-      <c r="I47" t="s">
-        <v>58</v>
-      </c>
-      <c r="L47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switching from different sequences to one to ensure the uniqueness of the IDs across the database
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
+++ b/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BE378C-3D61-40A1-B77E-54E64AB91BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640"/>
   </bookViews>
   <sheets>
     <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
@@ -20,12 +19,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="C33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="C33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="F33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -75,37 +74,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="G33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Sequenz immer an die Spalte [Resource]_[Postfix]_id mit ALTER TABLE / GRANT USAGE ON seq to USER
-oder eben keine Sequenz</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
   <si>
     <t>10_cre_table_raw_cds2db_in.sql</t>
   </si>
@@ -173,9 +147,6 @@
     <t>cds2db_in</t>
   </si>
   <si>
-    <t>cds2db_in_seq</t>
-  </si>
-  <si>
     <t>db_user</t>
   </si>
   <si>
@@ -183,9 +154,6 @@
   </si>
   <si>
     <t>db_log</t>
-  </si>
-  <si>
-    <t>db_log_seq</t>
   </si>
   <si>
     <t>cds2db_out</t>
@@ -302,7 +270,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -652,11 +620,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD35"/>
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,28 +634,28 @@
     <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -695,83 +663,83 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -800,7 +768,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B23" s="2"/>
     </row>
@@ -818,45 +786,45 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B29" s="2"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="D33" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>18</v>
@@ -865,39 +833,36 @@
         <v>19</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="L33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M33" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M33" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="N33" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
         <v>20</v>
@@ -909,75 +874,69 @@
         <v>1</v>
       </c>
       <c r="G34" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>2</v>
+      </c>
+      <c r="H35" t="s">
         <v>22</v>
       </c>
-      <c r="H34" t="s">
-        <v>2</v>
-      </c>
-      <c r="I34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H35" t="s">
-        <v>2</v>
-      </c>
-      <c r="I35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" t="s">
         <v>24</v>
-      </c>
-      <c r="D36" t="s">
-        <v>25</v>
       </c>
       <c r="F36" t="s">
         <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="H36" t="s">
+        <v>23</v>
+      </c>
+      <c r="I36" t="s">
+        <v>7</v>
+      </c>
+      <c r="J36" t="s">
+        <v>14</v>
+      </c>
+      <c r="K36" t="s">
+        <v>21</v>
+      </c>
+      <c r="L36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
         <v>2</v>
       </c>
-      <c r="I36" t="s">
-        <v>24</v>
-      </c>
-      <c r="J36" t="s">
-        <v>7</v>
-      </c>
-      <c r="K36" t="s">
-        <v>14</v>
-      </c>
-      <c r="L36" t="s">
-        <v>21</v>
-      </c>
-      <c r="M36" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H37" t="s">
-        <v>2</v>
-      </c>
-      <c r="I37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
         <v>20</v>
@@ -986,138 +945,132 @@
         <v>21</v>
       </c>
       <c r="G38" t="s">
+        <v>2</v>
+      </c>
+      <c r="H38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>2</v>
+      </c>
+      <c r="H39" t="s">
         <v>22</v>
       </c>
-      <c r="H38" t="s">
-        <v>2</v>
-      </c>
-      <c r="I38" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H39" t="s">
-        <v>2</v>
-      </c>
-      <c r="I39" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" t="s">
         <v>24</v>
       </c>
-      <c r="D40" t="s">
-        <v>25</v>
-      </c>
       <c r="G40" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="H40" t="s">
+        <v>23</v>
+      </c>
+      <c r="I40" t="s">
+        <v>13</v>
+      </c>
+      <c r="J40" t="s">
+        <v>15</v>
+      </c>
+      <c r="K40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
         <v>2</v>
       </c>
-      <c r="I40" t="s">
-        <v>24</v>
-      </c>
-      <c r="J40" t="s">
-        <v>13</v>
-      </c>
-      <c r="K40" t="s">
-        <v>15</v>
-      </c>
-      <c r="L40" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H41" t="s">
-        <v>2</v>
-      </c>
-      <c r="I41" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>4</v>
+      </c>
       <c r="H42" t="s">
-        <v>4</v>
-      </c>
-      <c r="I42" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C43" t="s">
         <v>20</v>
       </c>
       <c r="D43" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E43" t="s">
         <v>6</v>
       </c>
+      <c r="G43" t="s">
+        <v>4</v>
+      </c>
       <c r="H43" t="s">
+        <v>20</v>
+      </c>
+      <c r="K43" t="s">
+        <v>24</v>
+      </c>
+      <c r="L43" t="s">
+        <v>1</v>
+      </c>
+      <c r="M43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
         <v>4</v>
       </c>
-      <c r="I43" t="s">
-        <v>20</v>
-      </c>
-      <c r="L43" t="s">
-        <v>25</v>
-      </c>
-      <c r="M43" t="s">
-        <v>1</v>
-      </c>
-      <c r="N43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H44" t="s">
-        <v>4</v>
-      </c>
-      <c r="I44" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C45" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D45" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E45" t="s">
         <v>6</v>
       </c>
       <c r="F45" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="G45" t="s">
+        <v>4</v>
       </c>
       <c r="H45" t="s">
-        <v>4</v>
-      </c>
-      <c r="I45" t="s">
-        <v>57</v>
-      </c>
-      <c r="L45" t="s">
-        <v>25</v>
+        <v>55</v>
+      </c>
+      <c r="K45" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add function to check last check datetime in raw data and take over to core data if data is not chance
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
+++ b/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
   <si>
     <t>10_cre_table_raw_cds2db_in.sql</t>
   </si>
@@ -265,6 +265,15 @@
   </si>
   <si>
     <t>_all</t>
+  </si>
+  <si>
+    <t>20_take_over_check_date.sql</t>
+  </si>
+  <si>
+    <t>template_take_over_check_date_function.sql</t>
+  </si>
+  <si>
+    <t>take_over_last_check_date</t>
   </si>
 </sst>
 </file>
@@ -621,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N45"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,6 +1082,26 @@
         <v>24</v>
       </c>
     </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1</v>
+      </c>
+      <c r="I46" t="s">
+        <v>63</v>
+      </c>
+      <c r="J46" t="s">
+        <v>64</v>
+      </c>
+      <c r="K46" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
add template name for take over function
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
+++ b/Postgres-cds_hub/init/template/user_schema_rights_definition.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="65">
   <si>
     <t>10_cre_table_raw_cds2db_in.sql</t>
   </si>
@@ -633,7 +633,7 @@
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,6 +1086,9 @@
       <c r="A46" t="s">
         <v>62</v>
       </c>
+      <c r="B46" t="s">
+        <v>63</v>
+      </c>
       <c r="D46" t="s">
         <v>24</v>
       </c>

</xml_diff>